<commit_message>
adjusted the coordinates for the total value
</commit_message>
<xml_diff>
--- a/assets/resumo.xlsx
+++ b/assets/resumo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\resumo_valorizacao\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9AE97F-21CD-42EC-8516-80BF0887D003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179D80E9-D77A-4119-9366-972416E9B916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N509"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>